<commit_message>
Add import_data and UI
</commit_message>
<xml_diff>
--- a/struct.xlsx
+++ b/struct.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>ученики</t>
   </si>
@@ -68,9 +68,6 @@
     <t>11в</t>
   </si>
   <si>
-    <t>количество учеников</t>
-  </si>
-  <si>
     <t>[1, 3]</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t>log</t>
+  </si>
+  <si>
+    <t>id_учеников</t>
   </si>
 </sst>
 </file>
@@ -234,7 +234,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -267,19 +267,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -415,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -423,29 +410,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -728,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,6 +720,7 @@
     <col min="8" max="8" width="29.28515625" customWidth="1"/>
     <col min="9" max="9" width="19.140625" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
     <col min="13" max="13" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -754,12 +735,12 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="7"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="20"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -788,16 +769,10 @@
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="4" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
@@ -811,17 +786,11 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="K4" s="2">
-        <v>1</v>
+      <c r="K4" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M4" s="2">
-        <v>2</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
@@ -835,17 +804,11 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="K5" s="2">
-        <v>2</v>
+      <c r="K5" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" s="2">
-        <v>2</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -859,17 +822,11 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="K6" s="2">
-        <v>3</v>
+      <c r="K6" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M6" s="2">
-        <v>1</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
@@ -892,154 +849,154 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="12"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="F13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G15" s="12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F10" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="17" t="s">
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="F16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="I19" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="16"/>
+    </row>
+    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F21" s="6"/>
+      <c r="G21" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F11" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F12" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="11"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F14" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G15" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" s="10"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F16" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F17" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G18" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="8"/>
-      <c r="G19" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F20" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I20" s="19"/>
-    </row>
-    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F21" s="9"/>
-      <c r="G21" s="9" t="s">
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F22" s="6"/>
+      <c r="G22" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F22" s="9"/>
-      <c r="G22" s="9" t="s">
+    </row>
+    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F23" s="6"/>
+      <c r="G23" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F23" s="9"/>
-      <c r="G23" s="9" t="s">
+    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F24" s="6"/>
+      <c r="G24" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F24" s="9"/>
-      <c r="G24" s="9" t="s">
+    <row r="25" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="7"/>
+      <c r="G25" s="7" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="10"/>
-      <c r="G25" s="10" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:I2"/>
-    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>